<commit_message>
Figured out how to use consolidate
</commit_message>
<xml_diff>
--- a/Lambda4Unpivot.xlsx
+++ b/Lambda4Unpivot.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28803"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3882528B-73CF-4556-B526-5CE1E69A23AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F16DB9-0D70-4BE5-B00D-383330AB00EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Formats" sheetId="2" r:id="rId2"/>
-    <sheet name="Lists" sheetId="3" r:id="rId3"/>
+    <sheet name="Detail1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Report" sheetId="1" r:id="rId3"/>
+    <sheet name="Formats" sheetId="2" r:id="rId4"/>
+    <sheet name="Lists" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_fBCAST">_xlfn.LAMBDA(_xlpm._nData, _xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d, _xlfn.LET(_xlpm._c, COLUMNS(_xlpm._d) - 1, _xlfn.DROP(_xlfn.REDUCE("", _xlfn.TAKE(_xlpm._d, , 1), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.EXPAND(_xlpm.v, _xlpm._c, 1, _xlpm.v)))), 1))), _xlfn.HSTACK(_xlpm.f(_xlpm._nData), _xlfn.TOCOL(_xlfn.DROP(_xlpm._nData, , 1)))))</definedName>
@@ -35,7 +37,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -77,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="41">
   <si>
     <t>FROM:</t>
   </si>
@@ -182,6 +185,24 @@
   </si>
   <si>
     <t>Aircraft</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Details for Sum of Value</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -369,7 +390,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -384,6 +405,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -927,6 +954,54 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="mbieg" refreshedDate="45756.616702893516" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="72" xr:uid="{E3E73F7D-99E5-48A6-8B7B-53D5CD4E7B1B}">
+  <cacheSource type="consolidation">
+    <consolidation autoPage="0">
+      <rangeSets count="1">
+        <rangeSet ref="A22:G34" sheet="Report"/>
+      </rangeSets>
+    </consolidation>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Row" numFmtId="0">
+      <sharedItems count="12">
+        <s v="    C-43"/>
+        <s v="    C-45"/>
+        <s v="    C-46"/>
+        <s v="    C-54"/>
+        <s v="    C-61"/>
+        <s v="    C-64"/>
+        <s v="    C-69"/>
+        <s v="    C-78"/>
+        <s v="    C-87"/>
+        <s v="    DC-3 type"/>
+        <s v="    Lodestar type"/>
+        <s v="    Others"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Column" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1940" maxValue="1945" count="6">
+        <n v="1940"/>
+        <n v="1941"/>
+        <n v="1942"/>
+        <n v="1943"/>
+        <n v="1944"/>
+        <n v="1945"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Value" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4900"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="6">
   <r>
@@ -968,7 +1043,491 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="72">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="157"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="161"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="60"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1060"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="591"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="353"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1321"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="1423"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="72"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="356"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="635"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="147"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="209"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="454"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="82"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="187"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="2548"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="471"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="110"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="140"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="115"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="165"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="1057"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="2595"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <n v="4900"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="1491"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="180"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="297"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+    <m/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="5"/>
+    <n v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4417412-A609-4EC2-8B46-011F88C400E0}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:H17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
@@ -1059,6 +1618,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CFCA888-93B0-4D7B-A826-B6443E533AFC}" name="Table2" displayName="Table2" ref="A3:C75" totalsRowShown="0">
+  <autoFilter ref="A3:C75" xr:uid="{5CFCA888-93B0-4D7B-A826-B6443E533AFC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F6328429-FF70-46F2-B313-0700A62E3D81}" name="Row"/>
+    <tableColumn id="2" xr3:uid="{982FD3C9-03F0-43CE-B03A-B222FCE642CB}" name="Column"/>
+    <tableColumn id="3" xr3:uid="{9A01B5D7-F033-49BD-93C7-43720E718B8E}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33EBBF0F-200B-49A7-BE86-E02A26DD1F32}" name="_tSample" displayName="_tSample" ref="B7:E13" totalsRowShown="0">
   <autoFilter ref="B7:E13" xr:uid="{33EBBF0F-200B-49A7-BE86-E02A26DD1F32}"/>
   <tableColumns count="4">
@@ -1289,14 +1860,1143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA59135-DC3E-4787-A126-A23FF5A45D11}">
+  <dimension ref="A1:C75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1940</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>1942</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1943</v>
+      </c>
+      <c r="C7">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1944</v>
+      </c>
+      <c r="C8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1940</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>1941</v>
+      </c>
+      <c r="C11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>1943</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1944</v>
+      </c>
+      <c r="C14">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>1945</v>
+      </c>
+      <c r="C15">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>1941</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>1942</v>
+      </c>
+      <c r="C18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>1943</v>
+      </c>
+      <c r="C19">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>1944</v>
+      </c>
+      <c r="C20">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1945</v>
+      </c>
+      <c r="C21">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1942</v>
+      </c>
+      <c r="C24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1943</v>
+      </c>
+      <c r="C25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1944</v>
+      </c>
+      <c r="C26">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>1945</v>
+      </c>
+      <c r="C27">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>1940</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>1941</v>
+      </c>
+      <c r="C29">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>1942</v>
+      </c>
+      <c r="C30">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>1943</v>
+      </c>
+      <c r="C31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>1944</v>
+      </c>
+      <c r="C32">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <v>1941</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36">
+        <v>1942</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>1943</v>
+      </c>
+      <c r="C37">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38">
+        <v>1944</v>
+      </c>
+      <c r="C38">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39">
+        <v>1945</v>
+      </c>
+      <c r="C39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43">
+        <v>1943</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <v>1944</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>1945</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>1942</v>
+      </c>
+      <c r="C48">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49">
+        <v>1943</v>
+      </c>
+      <c r="C49">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>1944</v>
+      </c>
+      <c r="C50">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54">
+        <v>1942</v>
+      </c>
+      <c r="C54">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55">
+        <v>1943</v>
+      </c>
+      <c r="C55">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56">
+        <v>1944</v>
+      </c>
+      <c r="C56">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58">
+        <v>1940</v>
+      </c>
+      <c r="C58">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59">
+        <v>1941</v>
+      </c>
+      <c r="C59">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60">
+        <v>1942</v>
+      </c>
+      <c r="C60">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>1943</v>
+      </c>
+      <c r="C61">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62">
+        <v>1944</v>
+      </c>
+      <c r="C62">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63">
+        <v>1945</v>
+      </c>
+      <c r="C63">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64">
+        <v>1940</v>
+      </c>
+      <c r="C64">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65">
+        <v>1941</v>
+      </c>
+      <c r="C65">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66">
+        <v>1942</v>
+      </c>
+      <c r="C66">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67">
+        <v>1943</v>
+      </c>
+      <c r="C67">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70">
+        <v>1940</v>
+      </c>
+      <c r="C70">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71">
+        <v>1941</v>
+      </c>
+      <c r="C71">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72">
+        <v>1942</v>
+      </c>
+      <c r="C72">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73">
+        <v>1943</v>
+      </c>
+      <c r="C73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74">
+        <v>1944</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75">
+        <v>1945</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9894F598-6B82-4581-82F0-C7D063B6ECDD}">
+  <dimension ref="A3:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>1940</v>
+      </c>
+      <c r="C4">
+        <v>1941</v>
+      </c>
+      <c r="D4">
+        <v>1942</v>
+      </c>
+      <c r="E4">
+        <v>1943</v>
+      </c>
+      <c r="F4">
+        <v>1944</v>
+      </c>
+      <c r="G4">
+        <v>1945</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="13">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13">
+        <v>157</v>
+      </c>
+      <c r="F5" s="13">
+        <v>161</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13">
+        <v>19</v>
+      </c>
+      <c r="C6" s="13">
+        <v>41</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>60</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1060</v>
+      </c>
+      <c r="G6" s="13">
+        <v>591</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>46</v>
+      </c>
+      <c r="E7" s="13">
+        <v>353</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1321</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1423</v>
+      </c>
+      <c r="H7" s="13">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13">
+        <v>26</v>
+      </c>
+      <c r="E8" s="13">
+        <v>72</v>
+      </c>
+      <c r="F8" s="13">
+        <v>356</v>
+      </c>
+      <c r="G8" s="13">
+        <v>635</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13">
+        <v>51</v>
+      </c>
+      <c r="D9" s="13">
+        <v>147</v>
+      </c>
+      <c r="E9" s="13">
+        <v>400</v>
+      </c>
+      <c r="F9" s="13">
+        <v>400</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>209</v>
+      </c>
+      <c r="F10" s="13">
+        <v>454</v>
+      </c>
+      <c r="G10" s="13">
+        <v>82</v>
+      </c>
+      <c r="H10" s="13">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
+        <v>3</v>
+      </c>
+      <c r="G11" s="13">
+        <v>10</v>
+      </c>
+      <c r="H11" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13">
+        <v>187</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2548</v>
+      </c>
+      <c r="F12" s="13">
+        <v>471</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13">
+        <v>41</v>
+      </c>
+      <c r="E13" s="13">
+        <v>110</v>
+      </c>
+      <c r="F13" s="13">
+        <v>140</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="13">
+        <v>115</v>
+      </c>
+      <c r="C14" s="13">
+        <v>165</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1057</v>
+      </c>
+      <c r="E14" s="13">
+        <v>2595</v>
+      </c>
+      <c r="F14" s="13">
+        <v>4900</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1491</v>
+      </c>
+      <c r="H14" s="13">
+        <v>10323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="13">
+        <v>45</v>
+      </c>
+      <c r="C15" s="13">
+        <v>98</v>
+      </c>
+      <c r="D15" s="13">
+        <v>180</v>
+      </c>
+      <c r="E15" s="13">
+        <v>297</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="13">
+        <v>36</v>
+      </c>
+      <c r="C16" s="13">
+        <v>36</v>
+      </c>
+      <c r="D16" s="13">
+        <v>26</v>
+      </c>
+      <c r="E16" s="13">
+        <v>15</v>
+      </c>
+      <c r="F16" s="13">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>4</v>
+      </c>
+      <c r="H16" s="13">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="13">
+        <v>233</v>
+      </c>
+      <c r="C17" s="13">
+        <v>398</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1738</v>
+      </c>
+      <c r="E17" s="13">
+        <v>6817</v>
+      </c>
+      <c r="F17" s="13">
+        <v>9276</v>
+      </c>
+      <c r="G17" s="13">
+        <v>4236</v>
+      </c>
+      <c r="H17" s="13">
+        <v>22698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
   <dimension ref="A4:BB115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1612,6 +3312,11 @@
         <v>127</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1940</v>
@@ -4131,12 +5836,15 @@
       <dataRef ref="A7:G19" sheet="Report"/>
     </dataRefs>
   </dataConsolidate>
+  <hyperlinks>
+    <hyperlink ref="I21" r:id="rId1" xr:uid="{61E5376E-9383-4DDD-A93C-4016B9FBDE45}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -4174,7 +5882,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>08-Apr-2025</v>
+        <v>09-Apr-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4435,7 +6143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -4470,7 +6178,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>08-Apr-2025</v>
+        <v>09-Apr-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Documented the consolidate solution
</commit_message>
<xml_diff>
--- a/Lambda4Unpivot.xlsx
+++ b/Lambda4Unpivot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F16DB9-0D70-4BE5-B00D-383330AB00EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40E698-FDFC-489F-8D32-52AAA0A214D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail1" sheetId="5" r:id="rId1"/>
@@ -37,8 +37,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
-    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="5" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="43">
   <si>
     <t>FROM:</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Result of consolidation</t>
+  </si>
+  <si>
+    <t>Double click on grand total to get all data</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -408,7 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
@@ -1409,7 +1414,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4417412-A609-4EC2-8B46-011F88C400E0}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4417412-A609-4EC2-8B46-011F88C400E0}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -1528,7 +1533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1875,7 +1880,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2635,10 +2640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9894F598-6B82-4581-82F0-C7D063B6ECDD}">
-  <dimension ref="A3:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2649,6 +2654,11 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
@@ -2687,21 +2697,19 @@
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13">
+      <c r="D5">
         <v>27</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5">
         <v>157</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5">
         <v>161</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13">
+      <c r="H5">
         <v>352</v>
       </c>
     </row>
@@ -2709,23 +2717,22 @@
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6">
         <v>19</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6">
         <v>41</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13">
+      <c r="E6">
         <v>60</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6">
         <v>1060</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6">
         <v>591</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6">
         <v>1771</v>
       </c>
     </row>
@@ -2733,23 +2740,22 @@
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7">
         <v>46</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7">
         <v>353</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7">
         <v>1321</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7">
         <v>1423</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7">
         <v>3144</v>
       </c>
     </row>
@@ -2757,21 +2763,19 @@
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13">
+      <c r="D8">
         <v>26</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8">
         <v>72</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8">
         <v>356</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8">
         <v>635</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8">
         <v>1089</v>
       </c>
     </row>
@@ -2779,23 +2783,22 @@
       <c r="A9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9">
         <v>11</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9">
         <v>51</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9">
         <v>147</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9">
         <v>400</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9">
         <v>400</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13">
+      <c r="H9">
         <v>1009</v>
       </c>
     </row>
@@ -2803,23 +2806,22 @@
       <c r="A10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13">
+      <c r="C10">
         <v>6</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10">
         <v>209</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10">
         <v>454</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10">
         <v>82</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10">
         <v>752</v>
       </c>
     </row>
@@ -2827,19 +2829,16 @@
       <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11">
         <v>14</v>
       </c>
     </row>
@@ -2847,19 +2846,16 @@
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13">
+      <c r="D12">
         <v>187</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12">
         <v>2548</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12">
         <v>471</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13">
+      <c r="H12">
         <v>3206</v>
       </c>
     </row>
@@ -2867,19 +2863,16 @@
       <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13">
+      <c r="D13">
         <v>41</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13">
         <v>110</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13">
         <v>140</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13">
+      <c r="H13">
         <v>291</v>
       </c>
     </row>
@@ -2887,25 +2880,25 @@
       <c r="A14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14">
         <v>115</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14">
         <v>165</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14">
         <v>1057</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14">
         <v>2595</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14">
         <v>4900</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14">
         <v>1491</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14">
         <v>10323</v>
       </c>
     </row>
@@ -2913,21 +2906,19 @@
       <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15">
         <v>45</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15">
         <v>98</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15">
         <v>180</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15">
         <v>297</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13">
+      <c r="H15">
         <v>620</v>
       </c>
     </row>
@@ -2935,25 +2926,25 @@
       <c r="A16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16">
         <v>36</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16">
         <v>26</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16">
         <v>15</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16">
         <v>10</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16">
         <v>4</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16">
         <v>127</v>
       </c>
     </row>
@@ -2961,26 +2952,31 @@
       <c r="A17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17">
         <v>233</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17">
         <v>398</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17">
         <v>1738</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17">
         <v>6817</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17">
         <v>9276</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17">
         <v>4236</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17">
         <v>22698</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2995,7 +2991,7 @@
   </sheetPr>
   <dimension ref="A4:BB115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -3313,7 +3309,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="14" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>